<commit_message>
MCU PIM schematic update 2
</commit_message>
<xml_diff>
--- a/V1/Docs/MCU Board Pinout.xlsx
+++ b/V1/Docs/MCU Board Pinout.xlsx
@@ -5,18 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github\ACIM\INV\V1\V1\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Github\ACIM\INV\V1\V1\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A369684B-5F8D-49F0-935B-B7E5C2909A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B2C605-88FD-48FA-A9AC-532BE22E2F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{0F91A97A-6683-46BF-9321-4836F7AE917A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11220" activeTab="1" xr2:uid="{0F91A97A-6683-46BF-9321-4836F7AE917A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="V1" sheetId="1" r:id="rId1"/>
+    <sheet name="V0" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">V0!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'V1'!$A$1:$J$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="77">
   <si>
     <t>CH0</t>
   </si>
@@ -211,13 +213,70 @@
   </si>
   <si>
     <t>FUNCTION</t>
+  </si>
+  <si>
+    <t>MC_IU_SENSE</t>
+  </si>
+  <si>
+    <t>MC_IV_SENSE</t>
+  </si>
+  <si>
+    <t>MC_VDC_SENSE</t>
+  </si>
+  <si>
+    <t>MC_IDC_SENSE</t>
+  </si>
+  <si>
+    <t>MC_IW_SENSE</t>
+  </si>
+  <si>
+    <t>AN00</t>
+  </si>
+  <si>
+    <t>AN01</t>
+  </si>
+  <si>
+    <t>AN02</t>
+  </si>
+  <si>
+    <t>AN03</t>
+  </si>
+  <si>
+    <t>AN04</t>
+  </si>
+  <si>
+    <t>AN05</t>
+  </si>
+  <si>
+    <t>AN06</t>
+  </si>
+  <si>
+    <t>AN07</t>
+  </si>
+  <si>
+    <t>AN08</t>
+  </si>
+  <si>
+    <t>AN09</t>
+  </si>
+  <si>
+    <t>MC_VU_SENSE</t>
+  </si>
+  <si>
+    <t>MC_VW_SENSE</t>
+  </si>
+  <si>
+    <t>MC_VV_SENSE</t>
+  </si>
+  <si>
+    <t>MC_IPM_TEMP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +292,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -285,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -312,6 +386,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -633,11 +722,11 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J27" sqref="A1:J27"/>
+      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1233,4 +1322,585 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25D423C6-78A4-431C-9AEC-5A33AD027EC6}">
+  <dimension ref="A1:J27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.7109375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>12</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="7"/>
+      <c r="I2" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>23</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>13</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>14</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>15</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>11</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>16</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>22</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>21</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>17</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="12"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>18</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="12"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>24</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="12"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>27</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="12"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>28</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J15" s="12"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>29</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>30</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="12"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>8</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J18" s="12"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>6</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J19" s="12"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>5</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J20" s="12"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>4</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J21" s="12"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>33</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J22" s="12"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>46</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J23" s="12"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>31</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J24" s="12"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>49</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J25" s="12"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>45</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J26" s="12"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>39</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J27" s="12"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:J1" xr:uid="{25D423C6-78A4-431C-9AEC-5A33AD027EC6}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J27">
+      <sortCondition ref="J1"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>